<commit_message>
riscv compile not finished
</commit_message>
<xml_diff>
--- a/figures/result5.xlsx
+++ b/figures/result5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sakakibara\monte-carlo-ray-tracer_approx\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08A6C30-7315-493F-BC59-2C0478B449F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D258F99-1382-4280-9E71-D51049FAF36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="5" xr2:uid="{31F97659-7F59-47E3-B467-703D677997C4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="12" activeTab="18" xr2:uid="{31F97659-7F59-47E3-B467-703D677997C4}"/>
   </bookViews>
   <sheets>
     <sheet name="【非IS】Sheet0" sheetId="7" r:id="rId1"/>
@@ -30,6 +30,8 @@
     <sheet name="Sheet9" sheetId="26" r:id="rId15"/>
     <sheet name="Sheet1" sheetId="27" r:id="rId16"/>
     <sheet name="Sheet1 (2)" sheetId="29" r:id="rId17"/>
+    <sheet name="Sheet2" sheetId="30" r:id="rId18"/>
+    <sheet name="Sheet3" sheetId="31" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="78">
   <si>
     <t>wc, spp=16+16, prob=0.5</t>
     <phoneticPr fontId="1"/>
@@ -726,6 +728,109 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>method9y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>代表値は「リアルタイムでの隣接8 pixel平均」</t>
+    <rPh sb="0" eb="2">
+      <t>ダイヒョウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>リンセツ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヘイキン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>大</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>小</t>
+    </r>
+    <rPh sb="1" eb="2">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RGB全て同じくらい</t>
+    <rPh sb="3" eb="4">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>RGB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>は大きい</t>
+    </r>
+    <rPh sb="4" eb="5">
+      <t>オオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gは小さい</t>
+    <rPh sb="2" eb="3">
+      <t>チイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RGBG全てほぼ同じ</t>
+    <rPh sb="4" eb="5">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -735,7 +840,7 @@
     <numFmt numFmtId="176" formatCode="0.0000"/>
     <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +943,17 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -868,7 +984,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -930,6 +1046,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4276,6 +4398,1159 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9488609375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90757493749999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87095562500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83746787499999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80643149999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.779516875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73162068749999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6936075625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66278581250000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63806574999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61858568749999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58799887500000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56748687499999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54238881250000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$6:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.969724457085549</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96957708567432099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96964955133943198</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96958349610503802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96959765644011797</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96960179316823203</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96965705117876599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96966614355810998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96970577874773201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96980931022433903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96977899602059503</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96984840422707397</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.96991750030076496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96997547772514803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97003114887085395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-27AA-44D7-9298-ECDBC285C5F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>jpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9488609375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90757493749999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87095562500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83746787499999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80643149999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.779516875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73162068749999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6936075625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66278581250000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63806574999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61858568749999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58799887500000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56748687499999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54238881250000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$6:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.97358256456845504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97343190504403398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97349637224254204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.973455433519678</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97342864739244095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97353113163751004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97349623481527903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97349103729281194</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97354665957912301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97370872648134299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97361084881030002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97366207359169499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97372198382188402</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.97377590029943895</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.97382573224334201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-27AA-44D7-9298-ECDBC285C5F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="219400448"/>
+        <c:axId val="93080960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="219400448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93080960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="93080960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219400448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9488609375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90757493749999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87095562500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83746787499999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80643149999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.779516875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73162068749999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6936075625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66278581250000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63806574999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61858568749999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58799887500000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56748687499999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54238881250000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$6:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>73.226794999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.819843000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.369783999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.313892999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.918886000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.801806999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77.400279999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.584419999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.431151999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.214922000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>77.029354999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>77.461856999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>77.692588000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>76.842089999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>76.874512999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD20-4F71-8B0B-615812DE47C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>jpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9488609375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90757493749999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87095562500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83746787499999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80643149999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.779516875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73162068749999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6936075625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66278581250000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63806574999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61858568749999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58799887500000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56748687499999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.54238881250000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$6:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>63.485987999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.071605000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.587941999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.498549999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.198774999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.854737</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.670128000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67.896568000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.707449999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.337714000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67.349885</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67.815325999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68.050415999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>67.225453999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67.280556000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD20-4F71-8B0B-615812DE47C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="224930336"/>
+        <c:axId val="213750400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="224930336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="213750400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="213750400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="224930336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -11253,6 +12528,86 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12645,6 +14000,1038 @@
 </file>
 
 <file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17732,6 +20119,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>202405</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>207168</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>659605</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8D30F87-0045-F614-0EC8-91DC9371B0F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>159543</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>616743</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60054A2-B5BF-1BBF-B1C7-B0410531537A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -23485,8 +25949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C2B469-AEF4-4B63-B31F-BCB37B1539E1}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -25706,10 +28170,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEA1694-F670-4BE0-A01F-7368306F0412}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -26747,6 +29211,86 @@
       <c r="G52" s="3">
         <v>63.946093750000003</v>
       </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="C61" s="1"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="C62" s="1"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="C63" s="1"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="C64" s="1"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+    </row>
+    <row r="65" spans="3:5">
+      <c r="C65" s="1"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="66" spans="3:5">
+      <c r="C66" s="1"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+    </row>
+    <row r="67" spans="3:5">
+      <c r="C67" s="1"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="3:5">
+      <c r="C68" s="1"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="3:5">
+      <c r="C69" s="1"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="3:5">
+      <c r="C70" s="1"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" spans="3:5">
+      <c r="C71" s="1"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+    </row>
+    <row r="72" spans="3:5">
+      <c r="C72" s="1"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="3:5">
+      <c r="C73" s="1"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -27036,8 +29580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0506C7E9-1C4A-49B6-993E-CFFC44986C0C}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -27564,6 +30108,905 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="F24:G24"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5097DB85-A8E2-4022-9B9B-E70F8DE058B6}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G5" activeCellId="2" sqref="C5:C20 E5:E20 G5:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <cols>
+    <col min="1" max="1" width="8.9375" customWidth="1"/>
+    <col min="2" max="2" width="17.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.8125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f>1-B6/(1000*1000*16)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.969724457085549</v>
+      </c>
+      <c r="E6" s="3">
+        <v>73.226794999999996</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.97358256456845504</v>
+      </c>
+      <c r="G6" s="3">
+        <v>63.485987999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>818225</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C11" si="0">1-B7/(1000*1000*16)</f>
+        <v>0.9488609375</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.96957708567432099</v>
+      </c>
+      <c r="E7" s="3">
+        <v>75.819843000000006</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.97343190504403398</v>
+      </c>
+      <c r="G7" s="3">
+        <v>66.071605000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1478801</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90757493749999996</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.96964955133943198</v>
+      </c>
+      <c r="E8" s="3">
+        <v>77.369783999999996</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.97349637224254204</v>
+      </c>
+      <c r="G8" s="3">
+        <v>67.587941999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2064710</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.87095562500000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.96958349610503802</v>
+      </c>
+      <c r="E9" s="3">
+        <v>77.313892999999993</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.973455433519678</v>
+      </c>
+      <c r="G9" s="3">
+        <v>67.498549999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2600514</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83746787499999997</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.96959765644011797</v>
+      </c>
+      <c r="E10" s="3">
+        <v>76.918886000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.97342864739244095</v>
+      </c>
+      <c r="G10" s="3">
+        <v>67.198774999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3097096</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.80643149999999997</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.96960179316823203</v>
+      </c>
+      <c r="E11" s="3">
+        <v>77.801806999999997</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.97353113163751004</v>
+      </c>
+      <c r="G11" s="3">
+        <v>67.854737</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>3527730</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" ref="C9:C12" si="1">1-B12/(1000*1000*16)</f>
+        <v>0.779516875</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.96965705117876599</v>
+      </c>
+      <c r="E12" s="3">
+        <v>77.400279999999995</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.97349623481527903</v>
+      </c>
+      <c r="G12" s="3">
+        <v>67.670128000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>4294069</v>
+      </c>
+      <c r="C13" s="1">
+        <f>1-B13/(1000*1000*16)</f>
+        <v>0.73162068749999998</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.96966614355810998</v>
+      </c>
+      <c r="E13" s="3">
+        <v>77.584419999999994</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.97349103729281194</v>
+      </c>
+      <c r="G13" s="3">
+        <v>67.896568000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>4902279</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:C24" si="2">1-B14/(1000*1000*16)</f>
+        <v>0.6936075625</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.96970577874773201</v>
+      </c>
+      <c r="E14" s="3">
+        <v>78.431151999999997</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.97354665957912301</v>
+      </c>
+      <c r="G14" s="3">
+        <v>68.707449999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>5395427</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.66278581250000002</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.96980931022433903</v>
+      </c>
+      <c r="E15" s="3">
+        <v>77.214922000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.97370872648134299</v>
+      </c>
+      <c r="G15" s="3">
+        <v>67.337714000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>5790948</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.63806574999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.96977899602059503</v>
+      </c>
+      <c r="E16" s="3">
+        <v>77.029354999999995</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.97361084881030002</v>
+      </c>
+      <c r="G16" s="3">
+        <v>67.349885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>6102629</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61858568749999998</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.96984840422707397</v>
+      </c>
+      <c r="E17" s="3">
+        <v>77.461856999999995</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.97366207359169499</v>
+      </c>
+      <c r="G17" s="3">
+        <v>67.815325999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>6592018</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.58799887500000003</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.96991750030076496</v>
+      </c>
+      <c r="E18" s="3">
+        <v>77.692588000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.97372198382188402</v>
+      </c>
+      <c r="G18" s="3">
+        <v>68.050415999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>6920210</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.56748687499999995</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.96997547772514803</v>
+      </c>
+      <c r="E19" s="3">
+        <v>76.842089999999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.97377590029943895</v>
+      </c>
+      <c r="G19" s="3">
+        <v>67.225453999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>64</v>
+      </c>
+      <c r="B20">
+        <v>7321779</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.54238881250000004</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.97003114887085395</v>
+      </c>
+      <c r="E20" s="3">
+        <v>76.874512999999993</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.97382573224334201</v>
+      </c>
+      <c r="G20" s="3">
+        <v>67.280556000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="C21" s="1"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="C22" s="1"/>
+      <c r="D22" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="C23" s="1"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="C24" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34D6FD7-2A7F-47BC-8CBB-58BB55A4E976}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <cols>
+    <col min="2" max="2" width="17.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.8125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f>1-B6/(960*720*16)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.98458180013982499</v>
+      </c>
+      <c r="E6" s="3">
+        <v>63.269739583333298</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.98786103473815201</v>
+      </c>
+      <c r="G6" s="3">
+        <v>49.989978298611099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>629411</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C9" si="0">1-B7/(960*720*16)</f>
+        <v>0.94308711299189818</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.98473032397665206</v>
+      </c>
+      <c r="E7" s="3">
+        <v>63.074826388888802</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.98795833091970198</v>
+      </c>
+      <c r="G7" s="3">
+        <v>49.969846643518501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1187136</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89265625000000004</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.98452021713930205</v>
+      </c>
+      <c r="E8" s="3">
+        <v>64.003585069444398</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.98774347111498295</v>
+      </c>
+      <c r="G8" s="3">
+        <v>50.942375578703697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1686029</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84754512080439814</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.98461180814372096</v>
+      </c>
+      <c r="E9" s="3">
+        <v>63.943243634259197</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.98787522308369902</v>
+      </c>
+      <c r="G9" s="3">
+        <v>50.695379050925901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>2124346</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" ref="C10:C19" si="1">1-B10/(960*720*16)</f>
+        <v>0.80791142216435186</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.98459062796316599</v>
+      </c>
+      <c r="E10" s="3">
+        <v>64.119787326388803</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.98781013271662699</v>
+      </c>
+      <c r="G10" s="3">
+        <v>51.056997974536998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2519910</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77214355468749996</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.98459145271399895</v>
+      </c>
+      <c r="E11" s="3">
+        <v>64.630837673611097</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.98780153365744305</v>
+      </c>
+      <c r="G11" s="3">
+        <v>51.616426504629601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>2860984</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.741302806712963</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.98454395009492801</v>
+      </c>
+      <c r="E12" s="3">
+        <v>65.518475115740699</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.98775209470810699</v>
+      </c>
+      <c r="G12" s="3">
+        <v>52.480675636573999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>3141941</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71589798538773142</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.98447835378542903</v>
+      </c>
+      <c r="E13" s="3">
+        <v>65.996630497685103</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.98771695611164601</v>
+      </c>
+      <c r="G13" s="3">
+        <v>52.853275462962898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>3395852</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.69293872974537041</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.98463702830428101</v>
+      </c>
+      <c r="E14" s="3">
+        <v>65.721691261573994</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.98784538546299006</v>
+      </c>
+      <c r="G14" s="3">
+        <v>52.706934317129601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>3796911</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65667399088541667</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.98449900801503298</v>
+      </c>
+      <c r="E15" s="3">
+        <v>66.471506076388806</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.98768829637420397</v>
+      </c>
+      <c r="G15" s="3">
+        <v>53.504524016203703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>4117485</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.62768690321180554</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.98468512555076404</v>
+      </c>
+      <c r="E16" s="3">
+        <v>66.017255497685099</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.98784925438629001</v>
+      </c>
+      <c r="G16" s="3">
+        <v>53.164007523148101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4535204</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58991572627314814</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.98459785149389401</v>
+      </c>
+      <c r="E17" s="3">
+        <v>66.638310185185105</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.98774530706587305</v>
+      </c>
+      <c r="G17" s="3">
+        <v>53.839936342592502</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>4815526</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.56456832320601857</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.98448980409640097</v>
+      </c>
+      <c r="E18" s="3">
+        <v>67.884989872685097</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.98768588512262301</v>
+      </c>
+      <c r="G18" s="3">
+        <v>54.887450810185101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>4985569</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5491926179108797</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.98464062574702005</v>
+      </c>
+      <c r="E19" s="3">
+        <v>67.428744212962897</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.98777936942562605</v>
+      </c>
+      <c r="G19" s="3">
+        <v>54.670412326388799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="C20" s="1"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="C21" s="1"/>
+      <c r="D21" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="D22" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30218,7 +33661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC91EF9-5A2B-4E8B-B14F-BA82F77DFE6C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -30630,7 +34073,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -31304,7 +34747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3FC7A4-D7CA-4D5B-AB0C-26A064F79098}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>